<commit_message>
Everything working as it should
</commit_message>
<xml_diff>
--- a/data/excel_files_reduced/test_excel_4_reduced.xlsx
+++ b/data/excel_files_reduced/test_excel_4_reduced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrislittle/GitHub/speedsheet/excel-2-python/data/excel_files_reduced/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E94101A-7FD1-6D43-8BAA-B7252864AB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DD9833-51F4-BF47-A8F0-957A641D93AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -739,7 +739,7 @@
         <v>1-1.195217191</v>
       </c>
       <c r="Q3" t="str">
-        <f>LEFT(A3, 3)</f>
+        <f>LEFT(A3, 2)</f>
         <v>1</v>
       </c>
       <c r="R3" t="str">

</xml_diff>

<commit_message>
Test excel 4 works
</commit_message>
<xml_diff>
--- a/data/excel_files_reduced/test_excel_4_reduced.xlsx
+++ b/data/excel_files_reduced/test_excel_4_reduced.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrislittle/GitHub/speedsheet/excel-2-python/data/excel_files_reduced/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DD9833-51F4-BF47-A8F0-957A641D93AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ECE45D-86C3-DE49-8BA2-166F6389132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,30 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>A_id</t>
   </si>
@@ -123,9 +101,6 @@
     <t>Concatenate string</t>
   </si>
   <si>
-    <t>Conditional count</t>
-  </si>
-  <si>
     <t>Index value</t>
   </si>
   <si>
@@ -135,7 +110,7 @@
     <t>Rounded Ripeness</t>
   </si>
   <si>
-    <t>Fun Substitute</t>
+    <t>Replace</t>
   </si>
 </sst>
 </file>
@@ -499,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -510,7 +485,7 @@
     <col min="1" max="1" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +544,7 @@
         <v>21</v>
       </c>
       <c r="T1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U1" t="s">
         <v>24</v>
@@ -577,20 +552,17 @@
       <c r="V1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" t="s">
-        <v>26</v>
+      <c r="X1" t="s">
+        <v>8</v>
       </c>
       <c r="Y1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="Z1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -656,35 +628,31 @@
         <f>CONCATENATE(LEFT(I2,2),RIGHT(I2,2))</f>
         <v>good</v>
       </c>
-      <c r="T2">
-        <f>COUNTIFS(H:H,"&lt;0",I:I,"good")</f>
-        <v>2</v>
-      </c>
-      <c r="U2" t="str">
+      <c r="T2" t="str">
         <f>TRIM(I2)</f>
         <v>good</v>
       </c>
-      <c r="V2">
+      <c r="U2">
         <f>ROUND(G2,6)</f>
         <v>0.32984000000000002</v>
       </c>
-      <c r="W2" t="str">
-        <f>SUBSTITUTE(S2,"g","fun")</f>
-        <v>funood</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="V2" t="str">
+        <f>REPLACE(S2,4,1,"f")</f>
+        <v>goof</v>
+      </c>
+      <c r="X2" t="s">
         <v>18</v>
       </c>
+      <c r="Y2">
+        <f>COUNTIF(I:I,X2)</f>
+        <v>2</v>
+      </c>
       <c r="Z2">
-        <f>COUNTIF(I:I,Y2)</f>
+        <f>INDEX(Y2:Y100,1,1)</f>
         <v>2</v>
       </c>
-      <c r="AA2" cm="1">
-        <f t="array" ref="AA2">INDEX(Z:Z,2,0)</f>
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -750,31 +718,27 @@
         <f t="shared" ref="S3" si="6">CONCATENATE(LEFT(I3,2),RIGHT(I3,2))</f>
         <v>good</v>
       </c>
-      <c r="T3">
-        <f t="shared" ref="T3" si="7">COUNTIFS(H:H,"&lt;0",I:I,"good")</f>
-        <v>2</v>
-      </c>
-      <c r="U3" t="str">
-        <f t="shared" ref="U3" si="8">TRIM(I3)</f>
+      <c r="T3" t="str">
+        <f>TRIM(I3)</f>
         <v>good</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3" si="9">ROUND(G3,6)</f>
+      <c r="U3">
+        <f>ROUND(G3,6)</f>
         <v>0.86753000000000002</v>
       </c>
-      <c r="W3" t="str">
-        <f t="shared" ref="W3" si="10">SUBSTITUTE(S3,"g","fun")</f>
-        <v>funood</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="V3" t="str">
+        <f t="shared" ref="V3" si="7">REPLACE(S3,4,1,"f")</f>
+        <v>goof</v>
+      </c>
+      <c r="X3" t="s">
         <v>19</v>
       </c>
+      <c r="Y3">
+        <f>COUNTIF(I:I,X3)</f>
+        <v>0</v>
+      </c>
       <c r="Z3">
-        <f t="shared" ref="Z3" si="11">COUNTIF(I:I,Y3)</f>
-        <v>0</v>
-      </c>
-      <c r="AA3" cm="1">
-        <f t="array" ref="AA3">INDEX(Z:Z,2,0)</f>
+        <f>INDEX(Y2:Y100,1,1)</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>